<commit_message>
feat: generar venta en mc
</commit_message>
<xml_diff>
--- a/src/assets/files/Plantilla_Productos.xlsx
+++ b/src/assets/files/Plantilla_Productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEX\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E78E76-919D-9849-A043-664CB83A9948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5F9C23-BCD6-461C-9566-AB4391E6D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22560" windowHeight="18880" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>CODIGO DE BARRAS</t>
   </si>
@@ -48,30 +48,6 @@
     <t>SUPPLI.</t>
   </si>
   <si>
-    <t>PRECIO ADQ.</t>
-  </si>
-  <si>
-    <t>CLIENTES FINALES</t>
-  </si>
-  <si>
-    <t>CLIENTES POR MAYOR</t>
-  </si>
-  <si>
-    <t>Precio A</t>
-  </si>
-  <si>
-    <t>Precio B</t>
-  </si>
-  <si>
-    <t>Precio C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio D </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio E </t>
-  </si>
-  <si>
     <t>PRECIO A</t>
   </si>
   <si>
@@ -81,12 +57,6 @@
     <t>PRECIO C</t>
   </si>
   <si>
-    <t xml:space="preserve">PRECIO D </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRECIO E </t>
-  </si>
-  <si>
     <t>8202100217186</t>
   </si>
   <si>
@@ -142,13 +112,19 @@
   </si>
   <si>
     <t>hola</t>
+  </si>
+  <si>
+    <t>PRECIO D</t>
+  </si>
+  <si>
+    <t>PRECIO E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,25 +160,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
@@ -216,7 +173,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,24 +182,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -303,34 +248,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -344,24 +265,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -379,31 +288,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -413,6 +307,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1406,41 +1306,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="24.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="17" style="7" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.85546875" style="3"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="17" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="36" customHeight="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1452,228 +1351,247 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="20"/>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="3" t="s">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8">
+        <v>450</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="9">
+        <v>4.9679999999999991</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8">
+        <v>400</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="9">
+        <v>6.0720000000000001</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8">
+        <v>250</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="9">
+        <v>5.1612000000000009</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8">
+        <v>250</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="9">
+        <v>5.7684000000000006</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8">
+        <v>250</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="9">
+        <v>5.7684000000000006</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="5" t="s">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="D9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8">
+        <v>250</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="9">
+        <v>3.9468000000000005</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="8">
+        <v>250</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1.0929599999999999</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8">
+        <v>200</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="9">
+        <v>3.5824800000000008</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="16">
-      <c r="B4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="12">
-        <v>450</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="13">
-        <v>4.9679999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="16">
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="12">
-        <v>400</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="13">
-        <v>6.0720000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16">
-      <c r="B6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="12">
-        <v>250</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="13">
-        <v>5.1612000000000009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="16">
-      <c r="B7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="12">
-        <v>250</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="13">
-        <v>5.7684000000000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="16">
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="12">
-        <v>250</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="13">
-        <v>5.7684000000000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16">
-      <c r="B9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="12">
-        <v>250</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="13">
-        <v>3.9468000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="16">
-      <c r="B10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12">
-        <v>250</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="13">
-        <v>1.0929599999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="16">
-      <c r="B11" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="12">
-        <v>200</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="13">
-        <v>3.5824800000000008</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="16">
-      <c r="B12" s="11" t="s">
+      <c r="E12" s="8">
+        <v>170</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="12">
-        <v>170</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="13">
+      <c r="H12" s="9">
         <v>2.3073600000000001</v>
       </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:M1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>

</xml_diff>